<commit_message>
Modifying the preadvise report excel template
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_preadvise.xlsx
+++ b/reports/templates/reportTemplate_preadvise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28313A7-A94A-40A1-9ADE-ED22410D6CB3}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3D1A7C-7079-4F2A-A53E-B23FA513F447}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="8520" yWindow="1590" windowWidth="20085" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
   <si>
     <t>Preadvise ID</t>
   </si>
@@ -495,24 +495,9 @@
     </r>
   </si>
   <si>
-    <t>related to the Central America &amp; Carribean region</t>
-  </si>
-  <si>
-    <t>related to the South America</t>
-  </si>
-  <si>
     <t>related to North America</t>
   </si>
   <si>
-    <t>related to the Southern, Eastern &amp; South-Eastern Asia</t>
-  </si>
-  <si>
-    <t>related to the Polynesia, Melanesia &amp; Micronesia</t>
-  </si>
-  <si>
-    <t>related to Australia &amp; New Zealand</t>
-  </si>
-  <si>
     <t>related to Middle Africa, Western Africa, Eastern Africa</t>
   </si>
   <si>
@@ -526,6 +511,39 @@
   </si>
   <si>
     <t>If applicable (Only for prospects with an "Air &amp; Ocean" history):</t>
+  </si>
+  <si>
+    <t>related to the Southern, Eastern, South-Eastern Asia &amp; Melanesia</t>
+  </si>
+  <si>
+    <t>related to Australia, New Zealand, Polynesia &amp; Micronesia</t>
+  </si>
+  <si>
+    <t>related to Northern Europe</t>
+  </si>
+  <si>
+    <t>related to Southern Europe</t>
+  </si>
+  <si>
+    <t>related to Western Europe</t>
+  </si>
+  <si>
+    <t>related to Western Asia</t>
+  </si>
+  <si>
+    <t>related to Central Asia</t>
+  </si>
+  <si>
+    <t>related to Southern Africa</t>
+  </si>
+  <si>
+    <t>related to South America</t>
+  </si>
+  <si>
+    <t>related to Central America &amp; the Carribeans</t>
+  </si>
+  <si>
+    <t>related to Eastern Europe</t>
   </si>
 </sst>
 </file>
@@ -1079,16 +1097,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="1" max="1" width="53.875" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
     <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
     <col min="9" max="14" width="17.25" customWidth="1"/>
   </cols>
@@ -1125,7 +1143,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="I3" s="24" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
@@ -1352,7 +1370,7 @@
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="I14" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
@@ -1367,7 +1385,10 @@
       <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <f>COUNTIF(Data!G2:G1048576,"AM")</f>
+        <v>0</v>
+      </c>
       <c r="D15" s="6">
         <f>$B15/$B$10</f>
         <v>0</v>
@@ -1380,7 +1401,10 @@
       <c r="A16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <f>COUNTIF(Data!G2:G1048576,"AP")</f>
+        <v>0</v>
+      </c>
       <c r="D16" s="6">
         <f>$B16/$B$10</f>
         <v>0</v>
@@ -1408,7 +1432,10 @@
       <c r="A17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <f>COUNTIF(Data!G2:G1048576,"EU")</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="6">
         <f>$B17/$B$10</f>
         <v>0</v>
@@ -1420,23 +1447,23 @@
         <v>72</v>
       </c>
       <c r="J17" s="18">
-        <f>J6/$B$10</f>
+        <f t="shared" ref="J17:N21" si="0">J6/$B$10</f>
         <v>0</v>
       </c>
       <c r="K17" s="19">
-        <f>K6/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L17" s="19">
-        <f>L6/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M17" s="19">
-        <f>M6/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N17" s="20">
-        <f>N6/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1446,23 +1473,23 @@
         <v>73</v>
       </c>
       <c r="J18" s="18">
-        <f>J7/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18" s="19">
-        <f>K7/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L18" s="19">
-        <f>L7/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M18" s="19">
-        <f>M7/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N18" s="20">
-        <f>N7/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1470,9 +1497,12 @@
       <c r="A19" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <f>COUNTIFS(Data!H2:H1048576,"North America",Data!H2:H1048576,"")</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="6">
-        <f t="shared" ref="D19:D24" si="0">$B19/$B$10</f>
+        <f t="shared" ref="D19:D32" si="1">$B19/$B$10</f>
         <v>0</v>
       </c>
       <c r="E19" t="s">
@@ -1482,33 +1512,36 @@
         <v>74</v>
       </c>
       <c r="J19" s="18">
-        <f>J8/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K19" s="19">
-        <f>K8/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L19" s="19">
-        <f>L8/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M19" s="19">
-        <f>M8/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19" s="20">
-        <f>N8/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="B20" s="1">
+        <f>COUNTIFS(Data!H2:H1048576,"Central America",Data!H2:H1048576,"Caribbean")</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E20" t="s">
@@ -1518,33 +1551,36 @@
         <v>75</v>
       </c>
       <c r="J20" s="18">
-        <f>J9/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K20" s="19">
-        <f>K9/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20" s="19">
-        <f>L9/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M20" s="19">
-        <f>M9/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N20" s="20">
-        <f>N9/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="B21" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"South America")</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E21" t="s">
@@ -1554,33 +1590,36 @@
         <v>76</v>
       </c>
       <c r="J21" s="21">
-        <f>J10/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K21" s="22">
-        <f>K10/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L21" s="22">
-        <f>L10/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M21" s="22">
-        <f>M10/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N21" s="23">
-        <f>N10/$B$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="B22" s="1">
+        <f>COUNTIFS(Data!H2:H1048576,"Southern Asia",Data!H2:H1048576,"Eastern Asia",Data!H2:H1048576,"South-Eastern Asia",Data!H2:H1048576,"Melanesia")</f>
+        <v>0</v>
+      </c>
       <c r="D22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E22" t="s">
@@ -1589,11 +1628,14 @@
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="B23" s="1">
+        <f>COUNTIFS(Data!H2:H1048576,"Australia and New Zealand",Data!H2:H1048576,"Polynesia",Data!H2:H1048576,"Micronesia")</f>
+        <v>0</v>
+      </c>
       <c r="D23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E23" t="s">
@@ -1602,11 +1644,14 @@
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="B24" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Northern Europe")</f>
+        <v>0</v>
+      </c>
       <c r="D24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E24" t="s">
@@ -1615,75 +1660,159 @@
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="B25" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Southern Europe")</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="B26" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Western Europe")</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Eastern Europe")</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Western Asia")</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Central Asia")</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Northern Africa")</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="1">
+        <f>COUNTIFS(Data!H2:H1048576,"Middle Africa",Data!H2:H1048576,"Western Africa",Data!H2:H1048576,"Eastern Africa")</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Southern Africa")</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1">
-        <f>COUNTIF(Data!L2:L1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="6">
-        <f>$B36/$B$10</f>
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>70</v>
-      </c>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1">
-        <f>COUNTIF(Data!N2:N1048576,"Yes")</f>
+        <f>COUNTIF(Data!L2:L1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D37" s="6">
@@ -1696,10 +1825,10 @@
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1">
-        <f>COUNTIF(Data!P2:P1048576,"Yes")</f>
+        <f>COUNTIF(Data!N2:N1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D38" s="6">
@@ -1712,10 +1841,10 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1">
-        <f>COUNTIF(Data!R2:R1048576,"Yes")</f>
+        <f>COUNTIF(Data!P2:P1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D39" s="6">
@@ -1727,79 +1856,79 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="1">
+        <f>COUNTIF(Data!R2:R1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
+        <f>$B40/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B42" s="4">
         <f>SUM(Data!M2:M1048576)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B43" s="3">
         <f>SUM(Data!O2:O1048576)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B44" s="5">
         <f>SUM(Data!Q2:Q1048576)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B45" s="3">
         <f>SUM(Data!S2:S1048576)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="1">
-        <f>COUNTIF(Data!AS2:AS1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="D48" s="6">
-        <f>$B48/$B$10</f>
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>70</v>
-      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="1">
-        <f>COUNTIF(Data!AT2:AT1048576,"Yes")</f>
+        <f>COUNTIF(Data!AS2:AS1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D49" s="6">
@@ -1812,10 +1941,10 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="1">
-        <f>COUNTIF(Data!AU2:AU1048576,"Yes")</f>
+        <f>COUNTIF(Data!AT2:AT1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D50" s="6">
@@ -1828,10 +1957,10 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="1">
-        <f>COUNTIF(Data!AV2:AV1048576,"Yes")</f>
+        <f>COUNTIF(Data!AU2:AU1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D51" s="6">
@@ -1844,10 +1973,10 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1">
-        <f>COUNTIF(Data!AW2:AW1048576,"Yes")</f>
+        <f>COUNTIF(Data!AV2:AV1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D52" s="6">
@@ -1858,40 +1987,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="1">
+        <f>COUNTIF(Data!AW2:AW1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="6">
+        <f>$B53/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"A")</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="6">
-        <f>$B55/$B$10</f>
-        <v>0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>70</v>
-      </c>
+      <c r="A55" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"B")</f>
+        <f>COUNTIF(Data!AX2:AX1048576,"A")</f>
         <v>0</v>
       </c>
       <c r="D56" s="6">
@@ -1904,10 +2033,10 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B57" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"C")</f>
+        <f>COUNTIF(Data!AX2:AX1048576,"B")</f>
         <v>0</v>
       </c>
       <c r="D57" s="6">
@@ -1915,6 +2044,22 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="1">
+        <f>COUNTIF(Data!AX2:AX1048576,"C")</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="6">
+        <f>$B58/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1934,9 +2079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408FA63C-ED69-49C0-8A89-D58054A38125}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Adding the Excel report templates
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_preadvise.xlsx
+++ b/reports/templates/reportTemplate_preadvise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="495" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3D1A7C-7079-4F2A-A53E-B23FA513F447}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF48AF6-5B08-432E-BBE4-088947368604}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="1590" windowWidth="20085" windowHeight="11385" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; Ton(s)&quot;_-;\-* #,##0.00&quot; Ton(s)&quot;_-;_-* &quot;-&quot;??&quot; Ton(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00&quot; CMB(s)&quot;_-;\-* #,##0.00&quot; CBM(s)&quot;_-;_-* &quot;-&quot;??&quot; CBM(s)&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,11 +580,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="3"/>
-      <name val="Fira Code"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +593,12 @@
       <name val="Fira Sans"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Fira Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -779,20 +780,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyBorder="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyBorder="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -800,19 +799,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1097,21 +1126,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="53.875" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="60" customWidth="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1"/>
+    <col min="3" max="3" width="5.75" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="8" max="13" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1121,64 +1149,63 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="B5" s="1"/>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="M5" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1188,119 +1215,117 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="7" t="s">
+      <c r="H6" s="17" t="s">
         <v>72</v>
       </c>
+      <c r="I6" s="11">
+        <f>COUNTIF(Data!T2:T1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="J6" s="12">
-        <f>COUNTIF(Data!T2:T1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="13">
         <f>COUNTIF(Data!U2:U1048576,"Yes")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="13">
+      <c r="K6" s="12">
         <f>COUNTIF(Data!V2:V1048576,"Yes")</f>
         <v>0</v>
       </c>
+      <c r="L6" s="12">
+        <f>COUNTIF(Data!W2:W1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="M6" s="13">
-        <f>COUNTIF(Data!W2:W1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="14">
         <f>COUNTIF(Data!X2:X1048576,"Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B7" s="1"/>
-      <c r="I7" s="7" t="s">
+      <c r="H7" s="17" t="s">
         <v>73</v>
       </c>
+      <c r="I7" s="11">
+        <f>COUNTIF(Data!Y2:Y1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="J7" s="12">
-        <f>COUNTIF(Data!Y2:Y1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="13">
         <f>COUNTIF(Data!Z2:Z1048576,"Yes")</f>
         <v>0</v>
       </c>
-      <c r="L7" s="13">
+      <c r="K7" s="12">
         <f>COUNTIF(Data!AA2:AA1048576,"Yes")</f>
         <v>0</v>
       </c>
+      <c r="L7" s="12">
+        <f>COUNTIF(Data!AB2:AB1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="M7" s="13">
-        <f>COUNTIF(Data!AB2:AB1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="14">
         <f>COUNTIF(Data!AC2:AC1048576,"Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1">
+      <c r="A8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="17" t="s">
         <v>74</v>
       </c>
+      <c r="I8" s="11">
+        <f>COUNTIF(Data!AD2:AD1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="12">
-        <f>COUNTIF(Data!AD2:AD1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="13">
         <f>COUNTIF(Data!AE2:AE1048576,"Yes")</f>
         <v>0</v>
       </c>
-      <c r="L8" s="13">
+      <c r="K8" s="12">
         <f>COUNTIF(Data!AF2:AF1048576,"Yes")</f>
         <v>0</v>
       </c>
+      <c r="L8" s="12">
+        <f>COUNTIF(Data!AG2:AG1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="M8" s="13">
-        <f>COUNTIF(Data!AG2:AG1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="14">
         <f>COUNTIF(Data!AH2:AH1048576,"Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="B9" s="1"/>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="17" t="s">
         <v>75</v>
       </c>
+      <c r="I9" s="11">
+        <f>COUNTIF(Data!AI2:AI1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="J9" s="12">
-        <f>COUNTIF(Data!AI2:AI1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="13">
         <f>COUNTIF(Data!AJ2:AJ1048576,"Yes")</f>
         <v>0</v>
       </c>
-      <c r="L9" s="13">
+      <c r="K9" s="12">
         <f>COUNTIF(Data!AK2:AK1048576,"Yes")</f>
         <v>0</v>
       </c>
+      <c r="L9" s="12">
+        <f>COUNTIF(Data!AL2:AL1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="M9" s="13">
-        <f>COUNTIF(Data!AL2:AL1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="14">
         <f>COUNTIF(Data!AM2:AM1048576,"Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1308,34 +1333,34 @@
         <f>COUNTIF(Data!A2:A1048576,"&lt;&gt;"&amp;"")</f>
         <v>2</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="18" t="s">
         <v>76</v>
       </c>
+      <c r="I10" s="14">
+        <f>COUNTIF(Data!AN2:AN1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="15">
-        <f>COUNTIF(Data!AN2:AN1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="16">
         <f>COUNTIF(Data!AO2:AO1048576,"Yes")</f>
         <v>0</v>
       </c>
-      <c r="L10" s="16">
+      <c r="K10" s="15">
         <f>COUNTIF(Data!AP2:AP1048576,"Yes")</f>
         <v>0</v>
       </c>
+      <c r="L10" s="15">
+        <f>COUNTIF(Data!AQ2:AQ1048576,"Yes")</f>
+        <v>0</v>
+      </c>
       <c r="M10" s="16">
-        <f>COUNTIF(Data!AQ2:AQ1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="17">
         <f>COUNTIF(Data!AR2:AR1048576,"Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15" customHeight="1">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1351,7 +1376,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1367,21 +1392,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15" customHeight="1">
       <c r="B14" s="1"/>
-      <c r="I14" s="24" t="s">
+      <c r="H14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-    </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1397,7 +1422,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1412,23 +1437,23 @@
       <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="I16" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="K16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="L16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="M16" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1443,57 +1468,57 @@
       <c r="E17" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="H17" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J17" s="18">
-        <f t="shared" ref="J17:N21" si="0">J6/$B$10</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="19">
+      <c r="I17" s="19">
+        <f t="shared" ref="I17:M21" si="0">I6/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17" s="19">
+      <c r="K17" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M17" s="19">
+      <c r="L17" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="20">
+      <c r="M17" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="B18" s="1"/>
-      <c r="I18" s="7" t="s">
+      <c r="H18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="18">
+      <c r="I18" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="19">
+      <c r="J18" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18" s="19">
+      <c r="K18" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M18" s="19">
+      <c r="L18" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N18" s="20">
+      <c r="M18" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1508,31 +1533,31 @@
       <c r="E19" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="H19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J19" s="18">
+      <c r="I19" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="19">
+      <c r="J19" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="19">
+      <c r="K19" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M19" s="19">
+      <c r="L19" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="20">
+      <c r="M19" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1547,31 +1572,31 @@
       <c r="E20" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="H20" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="18">
+      <c r="I20" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="19">
+      <c r="J20" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="19">
+      <c r="K20" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M20" s="19">
+      <c r="L20" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N20" s="20">
+      <c r="M20" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1586,31 +1611,31 @@
       <c r="E21" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="H21" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="21">
+      <c r="I21" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="22">
+      <c r="J21" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" s="22">
+      <c r="K21" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M21" s="22">
+      <c r="L21" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N21" s="23">
+      <c r="M21" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1626,7 +1651,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1642,7 +1667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -1658,7 +1683,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1674,7 +1699,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1690,7 +1715,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1706,7 +1731,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15" customHeight="1">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1722,7 +1747,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -1738,7 +1763,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15" customHeight="1">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -1754,7 +1779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1770,7 +1795,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1786,28 +1811,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" customHeight="1">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" customHeight="1">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="A35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1823,7 +1847,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1839,7 +1863,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" customHeight="1">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1855,7 +1879,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" customHeight="1">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1871,10 +1895,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" customHeight="1">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" customHeight="1">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1883,7 +1907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15" customHeight="1">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1892,7 +1916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15" customHeight="1">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1901,7 +1925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" customHeight="1">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1910,20 +1934,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+    <row r="46" spans="1:7" ht="15" customHeight="1"/>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A47" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="15">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -1939,7 +1962,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1955,7 +1978,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1971,7 +1994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -1987,7 +2010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2003,19 +2026,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+    <row r="55" spans="1:7" ht="15">
+      <c r="A55" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2031,7 +2053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -2047,7 +2069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -2081,7 +2103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.375" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
@@ -2133,7 +2155,7 @@
     <col min="53" max="53" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2307,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2431,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Adding some modules and reorga. folder structure
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_preadvise.xlsx
+++ b/reports/templates/reportTemplate_preadvise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF48AF6-5B08-432E-BBE4-088947368604}"/>
+  <xr:revisionPtr revIDLastSave="518" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20CFFDF0-EF72-4BF3-A502-B2EFDAF89F8A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>Preadvise ID</t>
   </si>
@@ -545,6 +545,12 @@
   <si>
     <t>related to Eastern Europe</t>
   </si>
+  <si>
+    <t>Number of tenders involved in the following tradelanes</t>
+  </si>
+  <si>
+    <t>Share of tenders involved in the following tradelanes</t>
+  </si>
 </sst>
 </file>
 
@@ -555,7 +561,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; Ton(s)&quot;_-;\-* #,##0.00&quot; Ton(s)&quot;_-;_-* &quot;-&quot;??&quot; Ton(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00&quot; CMB(s)&quot;_-;\-* #,##0.00&quot; CBM(s)&quot;_-;_-* &quot;-&quot;??&quot; CBM(s)&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,7 +790,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1"/>
@@ -842,6 +848,7 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1128,9 +1135,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60" customWidth="1"/>
     <col min="2" max="2" width="24.25" customWidth="1"/>
@@ -1139,7 +1148,7 @@
     <col min="8" max="13" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1161,10 +1170,10 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1181,31 +1190,19 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="I5" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1">
+      <c r="H5" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1215,57 +1212,26 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="11">
-        <f>COUNTIF(Data!T2:T1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="12">
-        <f>COUNTIF(Data!U2:U1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <f>COUNTIF(Data!V2:V1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
-        <f>COUNTIF(Data!W2:W1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
-        <f>COUNTIF(Data!X2:X1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
-      <c r="H7" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="11">
-        <f>COUNTIF(Data!Y2:Y1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <f>COUNTIF(Data!Z2:Z1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
-        <f>COUNTIF(Data!AA2:AA1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="12">
-        <f>COUNTIF(Data!AB2:AB1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <f>COUNTIF(Data!AC2:AC1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1">
+      <c r="I7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>64</v>
       </c>
@@ -1276,56 +1242,56 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I8" s="11">
-        <f>COUNTIF(Data!AD2:AD1048576,"Yes")</f>
+        <f>COUNTIF(Data!T2:T1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="J8" s="12">
-        <f>COUNTIF(Data!AE2:AE1048576,"Yes")</f>
+        <f>COUNTIF(Data!U2:U1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="K8" s="12">
-        <f>COUNTIF(Data!AF2:AF1048576,"Yes")</f>
+        <f>COUNTIF(Data!V2:V1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="L8" s="12">
-        <f>COUNTIF(Data!AG2:AG1048576,"Yes")</f>
+        <f>COUNTIF(Data!W2:W1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="M8" s="13">
-        <f>COUNTIF(Data!AH2:AH1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1">
+        <f>COUNTIF(Data!X2:X1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="H9" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I9" s="11">
-        <f>COUNTIF(Data!AI2:AI1048576,"Yes")</f>
+        <f>COUNTIF(Data!Y2:Y1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="J9" s="12">
-        <f>COUNTIF(Data!AJ2:AJ1048576,"Yes")</f>
+        <f>COUNTIF(Data!Z2:Z1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="K9" s="12">
-        <f>COUNTIF(Data!AK2:AK1048576,"Yes")</f>
+        <f>COUNTIF(Data!AA2:AA1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="L9" s="12">
-        <f>COUNTIF(Data!AL2:AL1048576,"Yes")</f>
+        <f>COUNTIF(Data!AB2:AB1048576,"Yes")</f>
         <v>0</v>
       </c>
       <c r="M9" s="13">
-        <f>COUNTIF(Data!AM2:AM1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1">
+        <f>COUNTIF(Data!AC2:AC1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1333,34 +1299,57 @@
         <f>COUNTIF(Data!A2:A1048576,"&lt;&gt;"&amp;"")</f>
         <v>2</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="14">
-        <f>COUNTIF(Data!AN2:AN1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="15">
-        <f>COUNTIF(Data!AO2:AO1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <f>COUNTIF(Data!AP2:AP1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="15">
-        <f>COUNTIF(Data!AQ2:AQ1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="16">
-        <f>COUNTIF(Data!AR2:AR1048576,"Yes")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1">
+      <c r="H10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11">
+        <f>COUNTIF(Data!AD2:AD1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <f>COUNTIF(Data!AE2:AE1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f>COUNTIF(Data!AF2:AF1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f>COUNTIF(Data!AG2:AG1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="13">
+        <f>COUNTIF(Data!AH2:AH1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1">
+      <c r="H11" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="11">
+        <f>COUNTIF(Data!AI2:AI1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="12">
+        <f>COUNTIF(Data!AJ2:AJ1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <f>COUNTIF(Data!AK2:AK1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <f>COUNTIF(Data!AL2:AL1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <f>COUNTIF(Data!AM2:AM1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1375,8 +1364,31 @@
       <c r="E12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1">
+      <c r="H12" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="14">
+        <f>COUNTIF(Data!AN2:AN1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <f>COUNTIF(Data!AO2:AO1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="15">
+        <f>COUNTIF(Data!AP2:AP1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <f>COUNTIF(Data!AQ2:AQ1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="16">
+        <f>COUNTIF(Data!AR2:AR1048576,"Yes")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1392,21 +1404,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
-      <c r="H14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1437,23 +1438,19 @@
       <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="H16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1468,57 +1465,14 @@
       <c r="E17" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="19">
-        <f t="shared" ref="I17:M21" si="0">I6/$B$10</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="H18" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
+      <c r="H18" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1527,37 +1481,14 @@
         <v>0</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" ref="D19:D32" si="1">$B19/$B$10</f>
+        <f t="shared" ref="D19:D32" si="0">$B19/$B$10</f>
         <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1566,37 +1497,29 @@
         <v>0</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
+      <c r="I20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1605,37 +1528,37 @@
         <v>0</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
+      <c r="H21" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="19">
+        <f>I8/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="20">
+        <f>J8/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="20">
+        <f>K8/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="20">
+        <f>L8/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="21">
+        <f>M8/$B$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1644,14 +1567,37 @@
         <v>0</v>
       </c>
       <c r="D22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1">
+      <c r="H22" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="19">
+        <f>I9/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="20">
+        <f>J9/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="20">
+        <f>K9/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="20">
+        <f>L9/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="21">
+        <f>M9/$B$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1660,14 +1606,37 @@
         <v>0</v>
       </c>
       <c r="D23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
+      <c r="H23" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="19">
+        <f>I10/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
+        <f>J10/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <f>K10/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="20">
+        <f>L10/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="21">
+        <f>M10/$B$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -1676,14 +1645,37 @@
         <v>0</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1">
+      <c r="H24" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="19">
+        <f>I11/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="20">
+        <f>J11/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <f>K11/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
+        <f>L11/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="21">
+        <f>M11/$B$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1692,14 +1684,37 @@
         <v>0</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1">
+      <c r="H25" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="22">
+        <f>I12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="23">
+        <f>J12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="23">
+        <f>K12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="23">
+        <f>L12/$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="24">
+        <f>M12/$B$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1708,14 +1723,14 @@
         <v>0</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1724,14 +1739,14 @@
         <v>0</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1">
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1740,14 +1755,14 @@
         <v>0</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1">
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -1756,14 +1771,14 @@
         <v>0</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -1772,14 +1787,14 @@
         <v>0</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1">
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1788,14 +1803,14 @@
         <v>0</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1804,20 +1819,20 @@
         <v>0</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>65</v>
       </c>
@@ -1828,10 +1843,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1847,7 +1862,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1863,7 +1878,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1879,7 +1894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1895,10 +1910,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1907,7 +1922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1916,7 +1931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1934,8 +1949,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1"/>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>82</v>
       </c>
@@ -1946,7 +1961,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="15">
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -1962,7 +1977,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15">
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1978,7 +1993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15">
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1994,7 +2009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15">
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -2010,7 +2025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15">
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2026,7 +2041,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15">
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>96</v>
       </c>
@@ -2037,12 +2052,12 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:7" ht="15">
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
       <c r="B56" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"A")</f>
+        <f>COUNTIF(Data!AX2:AX1048576,"A-customer")</f>
         <v>0</v>
       </c>
       <c r="D56" s="6">
@@ -2053,12 +2068,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15">
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>89</v>
       </c>
       <c r="B57" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"B")</f>
+        <f>COUNTIF(Data!AX2:AX1048576,"B-customer")</f>
         <v>0</v>
       </c>
       <c r="D57" s="6">
@@ -2069,12 +2084,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15">
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>90</v>
       </c>
       <c r="B58" s="1">
-        <f>COUNTIF(Data!AX2:AX1048576,"C")</f>
+        <f>COUNTIF(Data!AX2:AX1048576,"C-customer")</f>
         <v>0</v>
       </c>
       <c r="D58" s="6">
@@ -2103,7 +2118,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.375" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
@@ -2155,7 +2170,7 @@
     <col min="53" max="53" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2322,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2453,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Correcting Excel preadvise template
</commit_message>
<xml_diff>
--- a/reports/templates/reportTemplate_preadvise.xlsx
+++ b/reports/templates/reportTemplate_preadvise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/Projet 02/moonshot/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="527" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD10EBF9-5221-47BC-8481-53027AB6BF2A}"/>
+  <xr:revisionPtr revIDLastSave="540" documentId="13_ncr:1_{BB587B11-3DD4-41F6-9455-588F5FC05102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{348B7D6B-B996-4A1A-8829-70E195F7B275}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{9DB76FDD-CFE2-43F9-8644-10A1BAD3A1A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
   <si>
     <t>Preadvise ID</t>
   </si>
@@ -554,6 +554,9 @@
   <si>
     <t>All</t>
   </si>
+  <si>
+    <t>related to Eastern Asia</t>
+  </si>
 </sst>
 </file>
 
@@ -564,7 +567,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; Ton(s)&quot;_-;\-* #,##0.00&quot; Ton(s)&quot;_-;_-* &quot;-&quot;??&quot; Ton(s)&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00&quot; CMB(s)&quot;_-;\-* #,##0.00&quot; CBM(s)&quot;_-;_-* &quot;-&quot;??&quot; CBM(s)&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,11 +1144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F65E63-F005-4CBF-AE0A-8C9CDC031092}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="40" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="60" customWidth="1"/>
     <col min="2" max="2" width="24.25" customWidth="1"/>
@@ -1156,7 +1159,7 @@
     <col min="16" max="16" width="4.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1178,10 +1181,10 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1200,7 +1203,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1208,13 +1211,13 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="B5" s="1"/>
       <c r="H5" s="25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1225,7 +1228,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" thickTop="1">
       <c r="B7" s="1"/>
       <c r="I7" s="8" t="s">
         <v>77</v>
@@ -1243,7 +1246,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>64</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="B9" s="1"/>
       <c r="H9" s="17" t="s">
         <v>73</v>
@@ -1303,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1">
       <c r="B11" s="1"/>
       <c r="H11" s="17" t="s">
         <v>75</v>
@@ -1361,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1416,10 +1419,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1462,7 +1465,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1478,29 +1481,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="B18" s="1"/>
       <c r="H18" s="25" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="1">
-        <f>COUNTIFS(Data!H2:H1048576,"North America",Data!H2:H1048576,"")</f>
+        <f>COUNTIFS(Data!H2:H1048576,"North America")</f>
         <v>0</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" ref="D19:D32" si="0">$B19/$B$10</f>
+        <f t="shared" ref="D19:D33" si="0">$B19/$B$10</f>
         <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" customHeight="1">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -1790,12 +1793,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" customHeight="1">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1">
-        <f>COUNTIF(Data!H2:H1048576,"Northern Africa")</f>
+        <f>COUNTIF(Data!H2:H1048576,"Eastern Asia")</f>
         <v>0</v>
       </c>
       <c r="D30" s="6">
@@ -1806,12 +1809,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B31" s="1">
-        <f>COUNTIFS(Data!H2:H1048576,"Middle Africa",Data!H2:H1048576,"Western Africa",Data!H2:H1048576,"Eastern Africa")</f>
+        <f>COUNTIF(Data!H2:H1048576,"Northern Africa")</f>
         <v>0</v>
       </c>
       <c r="D31" s="6">
@@ -1822,12 +1825,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1">
-        <f>COUNTIF(Data!H2:H1048576,"Southern Africa")</f>
+        <f>COUNTIFS(Data!H2:H1048576,"Middle Africa",Data!H2:H1048576,"Western Africa",Data!H2:H1048576,"Eastern Africa")</f>
         <v>0</v>
       </c>
       <c r="D32" s="6">
@@ -1838,13 +1841,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="1">
+        <f>COUNTIF(Data!H2:H1048576,"Southern Africa")</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="7" t="s">
         <v>65</v>
       </c>
@@ -1855,10 +1871,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1874,7 +1890,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1890,7 +1906,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15" customHeight="1">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1906,7 +1922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15" customHeight="1">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1922,10 +1938,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15" customHeight="1">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15" customHeight="1">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1934,7 +1950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15" customHeight="1">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1943,7 +1959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15" customHeight="1">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1952,7 +1968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="15" customHeight="1">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1961,8 +1977,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15" customHeight="1"/>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1">
       <c r="A47" s="7" t="s">
         <v>82</v>
       </c>
@@ -1973,7 +1989,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -1989,7 +2005,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -2021,7 +2037,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -2037,7 +2053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2053,7 +2069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15">
       <c r="A55" s="10" t="s">
         <v>96</v>
       </c>
@@ -2064,7 +2080,7 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2080,7 +2096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -2096,7 +2112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -2130,7 +2146,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.375" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
@@ -2182,7 +2198,7 @@
     <col min="53" max="53" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2334,7 +2350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2480,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>